<commit_message>
Update project configuration and dependencies and start writing drafts
</commit_message>
<xml_diff>
--- a/outputs/2023-11-21/2023-11-21_sem-fit-results-Rogoza.xlsx
+++ b/outputs/2023-11-21/2023-11-21_sem-fit-results-Rogoza.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="56">
   <si>
     <t>Dataset</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>GDIFF</t>
-  </si>
-  <si>
-    <t>p_pass</t>
   </si>
   <si>
     <t>CFI_pass</t>
@@ -542,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF69"/>
+  <dimension ref="A1:AE69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,19 +639,16 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32">
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>864</v>
@@ -734,25 +728,22 @@
       <c r="AC2" t="b">
         <v>1</v>
       </c>
-      <c r="AD2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>5</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
+      <c r="AD2">
+        <v>4</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>864</v>
@@ -827,30 +818,27 @@
         <v>1</v>
       </c>
       <c r="AB3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE3">
-        <v>4</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>3</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>864</v>
@@ -903,25 +891,22 @@
       <c r="AC4" t="b">
         <v>0</v>
       </c>
-      <c r="AD4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>864</v>
@@ -963,7 +948,7 @@
         <v>0.19</v>
       </c>
       <c r="Z5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="b">
         <v>0</v>
@@ -974,25 +959,22 @@
       <c r="AC5" t="b">
         <v>0</v>
       </c>
-      <c r="AD5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32">
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>809</v>
@@ -1072,25 +1054,22 @@
       <c r="AC6" t="b">
         <v>1</v>
       </c>
-      <c r="AD6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE6">
-        <v>5</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32">
+      <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>809</v>
@@ -1170,25 +1149,22 @@
       <c r="AC7" t="b">
         <v>1</v>
       </c>
-      <c r="AD7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE7">
-        <v>5</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32">
+      <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>809</v>
@@ -1230,7 +1206,7 @@
         <v>0.18</v>
       </c>
       <c r="Z8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="b">
         <v>0</v>
@@ -1241,25 +1217,22 @@
       <c r="AC8" t="b">
         <v>0</v>
       </c>
-      <c r="AD8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9">
         <v>809</v>
@@ -1301,7 +1274,7 @@
         <v>0.17</v>
       </c>
       <c r="Z9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" t="b">
         <v>0</v>
@@ -1312,25 +1285,22 @@
       <c r="AC9" t="b">
         <v>0</v>
       </c>
-      <c r="AD9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>1</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32">
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>1832</v>
@@ -1410,25 +1380,22 @@
       <c r="AC10" t="b">
         <v>1</v>
       </c>
-      <c r="AD10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE10">
-        <v>5</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32">
+      <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>1832</v>
@@ -1508,25 +1475,22 @@
       <c r="AC11" t="b">
         <v>1</v>
       </c>
-      <c r="AD11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE11">
-        <v>5</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32">
+      <c r="AD11">
+        <v>4</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>1832</v>
@@ -1568,7 +1532,7 @@
         <v>0.21</v>
       </c>
       <c r="Z12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA12" t="b">
         <v>0</v>
@@ -1579,25 +1543,22 @@
       <c r="AC12" t="b">
         <v>0</v>
       </c>
-      <c r="AD12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>1</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32">
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>1832</v>
@@ -1639,7 +1600,7 @@
         <v>0.19</v>
       </c>
       <c r="Z13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="b">
         <v>0</v>
@@ -1650,25 +1611,22 @@
       <c r="AC13" t="b">
         <v>0</v>
       </c>
-      <c r="AD13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>1</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32">
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14">
         <v>810</v>
@@ -1748,25 +1706,22 @@
       <c r="AC14" t="b">
         <v>1</v>
       </c>
-      <c r="AD14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE14">
-        <v>5</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32">
+      <c r="AD14">
+        <v>4</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>810</v>
@@ -1841,30 +1796,27 @@
         <v>1</v>
       </c>
       <c r="AB15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE15">
-        <v>4</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>3</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>810</v>
@@ -1909,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="AA16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB16" t="b">
         <v>0</v>
@@ -1917,25 +1869,22 @@
       <c r="AC16" t="b">
         <v>0</v>
       </c>
-      <c r="AD16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE16">
-        <v>2</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32">
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17">
         <v>810</v>
@@ -1977,7 +1926,7 @@
         <v>0.18</v>
       </c>
       <c r="Z17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
@@ -1988,25 +1937,22 @@
       <c r="AC17" t="b">
         <v>0</v>
       </c>
-      <c r="AD17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE17">
-        <v>1</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32">
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>810</v>
@@ -2086,25 +2032,22 @@
       <c r="AC18" t="b">
         <v>1</v>
       </c>
-      <c r="AD18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE18">
-        <v>5</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32">
+      <c r="AD18">
+        <v>4</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>810</v>
@@ -2184,25 +2127,22 @@
       <c r="AC19" t="b">
         <v>1</v>
       </c>
-      <c r="AD19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE19">
-        <v>5</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32">
+      <c r="AD19">
+        <v>4</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20">
         <v>810</v>
@@ -2244,7 +2184,7 @@
         <v>0.16</v>
       </c>
       <c r="Z20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA20" t="b">
         <v>0</v>
@@ -2255,25 +2195,22 @@
       <c r="AC20" t="b">
         <v>0</v>
       </c>
-      <c r="AD20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE20">
-        <v>1</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32">
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21">
         <v>810</v>
@@ -2315,7 +2252,7 @@
         <v>0.16</v>
       </c>
       <c r="Z21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA21" t="b">
         <v>0</v>
@@ -2326,25 +2263,22 @@
       <c r="AC21" t="b">
         <v>0</v>
       </c>
-      <c r="AD21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>1</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32">
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22">
         <v>891</v>
@@ -2424,25 +2358,22 @@
       <c r="AC22" t="b">
         <v>1</v>
       </c>
-      <c r="AD22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE22">
-        <v>5</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32">
+      <c r="AD22">
+        <v>4</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>891</v>
@@ -2517,30 +2448,27 @@
         <v>1</v>
       </c>
       <c r="AB23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC23" t="b">
         <v>0</v>
       </c>
-      <c r="AD23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>3</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32">
+      <c r="AD23">
+        <v>2</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>891</v>
@@ -2591,27 +2519,24 @@
         <v>1</v>
       </c>
       <c r="AC24" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>4</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>3</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25">
         <v>891</v>
@@ -2653,7 +2578,7 @@
         <v>0.16</v>
       </c>
       <c r="Z25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA25" t="b">
         <v>0</v>
@@ -2664,25 +2589,22 @@
       <c r="AC25" t="b">
         <v>0</v>
       </c>
-      <c r="AD25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE25">
-        <v>1</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32">
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26">
         <v>864</v>
@@ -2762,25 +2684,22 @@
       <c r="AC26" t="b">
         <v>1</v>
       </c>
-      <c r="AD26" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE26">
-        <v>5</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32">
+      <c r="AD26">
+        <v>4</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27">
         <v>864</v>
@@ -2855,30 +2774,27 @@
         <v>1</v>
       </c>
       <c r="AB27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD27" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE27">
-        <v>4</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>3</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28">
         <v>864</v>
@@ -2920,7 +2836,7 @@
         <v>0.29</v>
       </c>
       <c r="Z28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA28" t="b">
         <v>0</v>
@@ -2931,25 +2847,22 @@
       <c r="AC28" t="b">
         <v>0</v>
       </c>
-      <c r="AD28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <v>1</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32">
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29">
         <v>864</v>
@@ -2991,7 +2904,7 @@
         <v>0.27</v>
       </c>
       <c r="Z29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA29" t="b">
         <v>0</v>
@@ -3002,25 +2915,22 @@
       <c r="AC29" t="b">
         <v>0</v>
       </c>
-      <c r="AD29" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE29">
-        <v>1</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32">
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30">
         <v>891</v>
@@ -3100,25 +3010,22 @@
       <c r="AC30" t="b">
         <v>1</v>
       </c>
-      <c r="AD30" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE30">
-        <v>5</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32">
+      <c r="AD30">
+        <v>4</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31">
         <v>891</v>
@@ -3193,30 +3100,27 @@
         <v>1</v>
       </c>
       <c r="AB31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD31" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE31">
-        <v>4</v>
-      </c>
-      <c r="AF31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD31">
+        <v>3</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32">
         <v>891</v>
@@ -3258,7 +3162,7 @@
         <v>0.2</v>
       </c>
       <c r="Z32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA32" t="b">
         <v>0</v>
@@ -3269,25 +3173,22 @@
       <c r="AC32" t="b">
         <v>0</v>
       </c>
-      <c r="AD32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <v>1</v>
-      </c>
-      <c r="AF32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33">
         <v>891</v>
@@ -3329,7 +3230,7 @@
         <v>0.22</v>
       </c>
       <c r="Z33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA33" t="b">
         <v>0</v>
@@ -3340,25 +3241,22 @@
       <c r="AC33" t="b">
         <v>0</v>
       </c>
-      <c r="AD33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE33">
-        <v>1</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:32">
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34">
         <v>810</v>
@@ -3438,25 +3336,22 @@
       <c r="AC34" t="b">
         <v>1</v>
       </c>
-      <c r="AD34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE34">
-        <v>5</v>
-      </c>
-      <c r="AF34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:32">
+      <c r="AD34">
+        <v>4</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35">
         <v>810</v>
@@ -3536,25 +3431,22 @@
       <c r="AC35" t="b">
         <v>1</v>
       </c>
-      <c r="AD35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE35">
-        <v>5</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32">
+      <c r="AD35">
+        <v>4</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D36">
         <v>810</v>
@@ -3596,7 +3488,7 @@
         <v>0.2</v>
       </c>
       <c r="Z36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA36" t="b">
         <v>0</v>
@@ -3607,25 +3499,22 @@
       <c r="AC36" t="b">
         <v>0</v>
       </c>
-      <c r="AD36" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE36">
-        <v>1</v>
-      </c>
-      <c r="AF36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:32">
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37">
         <v>810</v>
@@ -3667,7 +3556,7 @@
         <v>0.2</v>
       </c>
       <c r="Z37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA37" t="b">
         <v>0</v>
@@ -3678,25 +3567,22 @@
       <c r="AC37" t="b">
         <v>0</v>
       </c>
-      <c r="AD37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE37">
-        <v>1</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:32">
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38">
         <v>917</v>
@@ -3776,25 +3662,22 @@
       <c r="AC38" t="b">
         <v>1</v>
       </c>
-      <c r="AD38" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE38">
-        <v>5</v>
-      </c>
-      <c r="AF38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:32">
+      <c r="AD38">
+        <v>4</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39">
         <v>917</v>
@@ -3863,36 +3746,33 @@
         <v>21.18</v>
       </c>
       <c r="Z39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC39" t="b">
         <v>0</v>
       </c>
-      <c r="AD39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE39">
-        <v>2</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32">
+      <c r="AD39">
+        <v>1</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40">
         <v>917</v>
@@ -3934,7 +3814,7 @@
         <v>0.2</v>
       </c>
       <c r="Z40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA40" t="b">
         <v>0</v>
@@ -3945,25 +3825,22 @@
       <c r="AC40" t="b">
         <v>0</v>
       </c>
-      <c r="AD40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE40">
-        <v>1</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32">
+      <c r="AD40">
+        <v>0</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41">
         <v>917</v>
@@ -4005,7 +3882,7 @@
         <v>0.22</v>
       </c>
       <c r="Z41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA41" t="b">
         <v>0</v>
@@ -4016,25 +3893,22 @@
       <c r="AC41" t="b">
         <v>0</v>
       </c>
-      <c r="AD41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE41">
-        <v>1</v>
-      </c>
-      <c r="AF41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32">
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D42">
         <v>810</v>
@@ -4114,25 +3988,22 @@
       <c r="AC42" t="b">
         <v>1</v>
       </c>
-      <c r="AD42" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE42">
-        <v>5</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:32">
+      <c r="AD42">
+        <v>4</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43">
         <v>810</v>
@@ -4212,25 +4083,22 @@
       <c r="AC43" t="b">
         <v>1</v>
       </c>
-      <c r="AD43" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE43">
-        <v>5</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32">
+      <c r="AD43">
+        <v>4</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D44">
         <v>810</v>
@@ -4272,7 +4140,7 @@
         <v>0.19</v>
       </c>
       <c r="Z44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA44" t="b">
         <v>0</v>
@@ -4283,25 +4151,22 @@
       <c r="AC44" t="b">
         <v>0</v>
       </c>
-      <c r="AD44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE44">
-        <v>1</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32">
+      <c r="AD44">
+        <v>0</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45">
         <v>810</v>
@@ -4343,7 +4208,7 @@
         <v>0.18</v>
       </c>
       <c r="Z45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA45" t="b">
         <v>0</v>
@@ -4354,25 +4219,22 @@
       <c r="AC45" t="b">
         <v>0</v>
       </c>
-      <c r="AD45" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE45">
-        <v>1</v>
-      </c>
-      <c r="AF45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32">
+      <c r="AD45">
+        <v>0</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D46">
         <v>864</v>
@@ -4452,25 +4314,22 @@
       <c r="AC46" t="b">
         <v>1</v>
       </c>
-      <c r="AD46" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE46">
-        <v>5</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32">
+      <c r="AD46">
+        <v>4</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47">
         <v>864</v>
@@ -4550,25 +4409,22 @@
       <c r="AC47" t="b">
         <v>1</v>
       </c>
-      <c r="AD47" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE47">
-        <v>5</v>
-      </c>
-      <c r="AF47" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32">
+      <c r="AD47">
+        <v>4</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D48">
         <v>864</v>
@@ -4610,7 +4466,7 @@
         <v>0.25</v>
       </c>
       <c r="Z48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA48" t="b">
         <v>0</v>
@@ -4621,25 +4477,22 @@
       <c r="AC48" t="b">
         <v>0</v>
       </c>
-      <c r="AD48" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE48">
-        <v>1</v>
-      </c>
-      <c r="AF48" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:32">
+      <c r="AD48">
+        <v>0</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49">
         <v>864</v>
@@ -4681,7 +4534,7 @@
         <v>0.26</v>
       </c>
       <c r="Z49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA49" t="b">
         <v>0</v>
@@ -4692,25 +4545,22 @@
       <c r="AC49" t="b">
         <v>0</v>
       </c>
-      <c r="AD49" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE49">
-        <v>1</v>
-      </c>
-      <c r="AF49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:32">
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50">
         <v>1890</v>
@@ -4790,25 +4640,22 @@
       <c r="AC50" t="b">
         <v>1</v>
       </c>
-      <c r="AD50" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE50">
-        <v>5</v>
-      </c>
-      <c r="AF50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:32">
+      <c r="AD50">
+        <v>4</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51">
         <v>1890</v>
@@ -4883,30 +4730,27 @@
         <v>1</v>
       </c>
       <c r="AB51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC51" t="b">
         <v>0</v>
       </c>
-      <c r="AD51" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE51">
-        <v>3</v>
-      </c>
-      <c r="AF51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:32">
+      <c r="AD51">
+        <v>2</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52">
         <v>1890</v>
@@ -4948,7 +4792,7 @@
         <v>0.19</v>
       </c>
       <c r="Z52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA52" t="b">
         <v>0</v>
@@ -4959,25 +4803,22 @@
       <c r="AC52" t="b">
         <v>0</v>
       </c>
-      <c r="AD52" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE52">
-        <v>1</v>
-      </c>
-      <c r="AF52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:32">
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53">
         <v>1890</v>
@@ -5019,7 +4860,7 @@
         <v>0.21</v>
       </c>
       <c r="Z53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA53" t="b">
         <v>0</v>
@@ -5030,25 +4871,22 @@
       <c r="AC53" t="b">
         <v>0</v>
       </c>
-      <c r="AD53" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE53">
-        <v>1</v>
-      </c>
-      <c r="AF53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:32">
+      <c r="AD53">
+        <v>0</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D54">
         <v>1647</v>
@@ -5128,25 +4966,22 @@
       <c r="AC54" t="b">
         <v>1</v>
       </c>
-      <c r="AD54" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE54">
-        <v>5</v>
-      </c>
-      <c r="AF54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:32">
+      <c r="AD54">
+        <v>4</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55">
         <v>1647</v>
@@ -5221,30 +5056,27 @@
         <v>1</v>
       </c>
       <c r="AB55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC55" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD55" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE55">
-        <v>4</v>
-      </c>
-      <c r="AF55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD55">
+        <v>3</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56">
         <v>1647</v>
@@ -5295,27 +5127,24 @@
         <v>1</v>
       </c>
       <c r="AC56" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD56" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE56">
-        <v>4</v>
-      </c>
-      <c r="AF56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:32">
+        <v>0</v>
+      </c>
+      <c r="AD56">
+        <v>3</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57">
         <v>1647</v>
@@ -5357,7 +5186,7 @@
         <v>0.15</v>
       </c>
       <c r="Z57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA57" t="b">
         <v>0</v>
@@ -5368,25 +5197,22 @@
       <c r="AC57" t="b">
         <v>0</v>
       </c>
-      <c r="AD57" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE57">
-        <v>1</v>
-      </c>
-      <c r="AF57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:32">
+      <c r="AD57">
+        <v>0</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D58">
         <v>945</v>
@@ -5466,25 +5292,22 @@
       <c r="AC58" t="b">
         <v>1</v>
       </c>
-      <c r="AD58" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE58">
-        <v>5</v>
-      </c>
-      <c r="AF58" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:32">
+      <c r="AD58">
+        <v>4</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D59">
         <v>945</v>
@@ -5559,30 +5382,27 @@
         <v>1</v>
       </c>
       <c r="AB59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC59" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD59" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE59">
-        <v>4</v>
-      </c>
-      <c r="AF59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD59">
+        <v>3</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D60">
         <v>945</v>
@@ -5624,7 +5444,7 @@
         <v>0.19</v>
       </c>
       <c r="Z60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA60" t="b">
         <v>0</v>
@@ -5635,25 +5455,22 @@
       <c r="AC60" t="b">
         <v>0</v>
       </c>
-      <c r="AD60" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE60">
-        <v>1</v>
-      </c>
-      <c r="AF60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:32">
+      <c r="AD60">
+        <v>0</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D61">
         <v>945</v>
@@ -5695,7 +5512,7 @@
         <v>0.18</v>
       </c>
       <c r="Z61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" t="b">
         <v>0</v>
@@ -5706,25 +5523,22 @@
       <c r="AC61" t="b">
         <v>0</v>
       </c>
-      <c r="AD61" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE61">
-        <v>1</v>
-      </c>
-      <c r="AF61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:32">
+      <c r="AD61">
+        <v>0</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D62">
         <v>918</v>
@@ -5804,25 +5618,22 @@
       <c r="AC62" t="b">
         <v>1</v>
       </c>
-      <c r="AD62" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE62">
-        <v>5</v>
-      </c>
-      <c r="AF62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:32">
+      <c r="AD62">
+        <v>4</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D63">
         <v>918</v>
@@ -5897,30 +5708,27 @@
         <v>1</v>
       </c>
       <c r="AB63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC63" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD63" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE63">
-        <v>4</v>
-      </c>
-      <c r="AF63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:32">
+        <v>1</v>
+      </c>
+      <c r="AD63">
+        <v>3</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D64">
         <v>918</v>
@@ -5962,7 +5770,7 @@
         <v>0.2</v>
       </c>
       <c r="Z64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA64" t="b">
         <v>0</v>
@@ -5973,25 +5781,22 @@
       <c r="AC64" t="b">
         <v>0</v>
       </c>
-      <c r="AD64" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE64">
-        <v>1</v>
-      </c>
-      <c r="AF64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:32">
+      <c r="AD64">
+        <v>0</v>
+      </c>
+      <c r="AE64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31">
       <c r="A65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D65">
         <v>918</v>
@@ -6033,7 +5838,7 @@
         <v>0.21</v>
       </c>
       <c r="Z65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA65" t="b">
         <v>0</v>
@@ -6044,25 +5849,22 @@
       <c r="AC65" t="b">
         <v>0</v>
       </c>
-      <c r="AD65" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE65">
-        <v>1</v>
-      </c>
-      <c r="AF65" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:32">
+      <c r="AD65">
+        <v>0</v>
+      </c>
+      <c r="AE65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" t="s">
         <v>49</v>
-      </c>
-      <c r="C66" t="s">
-        <v>50</v>
       </c>
       <c r="D66">
         <v>792</v>
@@ -6142,25 +5944,22 @@
       <c r="AC66" t="b">
         <v>1</v>
       </c>
-      <c r="AD66" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE66">
-        <v>5</v>
-      </c>
-      <c r="AF66" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:32">
+      <c r="AD66">
+        <v>4</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D67">
         <v>792</v>
@@ -6240,25 +6039,22 @@
       <c r="AC67" t="b">
         <v>1</v>
       </c>
-      <c r="AD67" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE67">
-        <v>5</v>
-      </c>
-      <c r="AF67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:32">
+      <c r="AD67">
+        <v>4</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D68">
         <v>792</v>
@@ -6300,7 +6096,7 @@
         <v>0.25</v>
       </c>
       <c r="Z68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA68" t="b">
         <v>0</v>
@@ -6311,25 +6107,22 @@
       <c r="AC68" t="b">
         <v>0</v>
       </c>
-      <c r="AD68" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE68">
-        <v>1</v>
-      </c>
-      <c r="AF68" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:32">
+      <c r="AD68">
+        <v>0</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D69">
         <v>792</v>
@@ -6371,7 +6164,7 @@
         <v>0.22</v>
       </c>
       <c r="Z69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA69" t="b">
         <v>0</v>
@@ -6382,14 +6175,11 @@
       <c r="AC69" t="b">
         <v>0</v>
       </c>
-      <c r="AD69" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE69">
-        <v>1</v>
-      </c>
-      <c r="AF69" t="s">
-        <v>56</v>
+      <c r="AD69">
+        <v>0</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>